<commit_message>
main docs update and GREGWT.r small update
</commit_message>
<xml_diff>
--- a/docs/example_be/data/Electricity_w_ConstructionYear_2025.xlsx
+++ b/docs/example_be/data/Electricity_w_ConstructionYear_2025.xlsx
@@ -14,9 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>ConstructionYear_1900</t>
+  </si>
+  <si>
+    <t>ConstructionYear_1918</t>
   </si>
   <si>
     <t>ConstructionYear_1945</t>
@@ -425,15 +428,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -471,204 +474,216 @@
       <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2">
-        <v>670</v>
-      </c>
-      <c r="C2">
-        <v>46595</v>
+        <v>14</v>
       </c>
       <c r="D2">
-        <v>22033</v>
+        <v>33418</v>
       </c>
       <c r="E2">
-        <v>22805</v>
+        <v>29831</v>
       </c>
       <c r="F2">
-        <v>47057</v>
+        <v>16378</v>
       </c>
       <c r="G2">
-        <v>40247</v>
+        <v>24107</v>
       </c>
       <c r="H2">
-        <v>26465</v>
+        <v>34345</v>
       </c>
       <c r="I2">
-        <v>21886</v>
+        <v>38718</v>
       </c>
       <c r="J2">
-        <v>13180</v>
+        <v>44712</v>
       </c>
       <c r="K2">
-        <v>15476</v>
+        <v>15356.31</v>
       </c>
       <c r="L2">
-        <v>23908</v>
+        <v>13317</v>
       </c>
       <c r="M2">
-        <v>12999</v>
+        <v>39565</v>
+      </c>
+      <c r="N2">
+        <v>22970</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3">
-        <v>3548</v>
+        <v>2656</v>
       </c>
       <c r="C3">
-        <v>30801</v>
+        <v>2107</v>
       </c>
       <c r="D3">
-        <v>25446</v>
+        <v>16546</v>
       </c>
       <c r="E3">
-        <v>20512</v>
+        <v>34296</v>
       </c>
       <c r="F3">
-        <v>48815</v>
+        <v>18102</v>
       </c>
       <c r="G3">
-        <v>43553</v>
+        <v>26041</v>
       </c>
       <c r="H3">
-        <v>31999</v>
+        <v>25023</v>
       </c>
       <c r="I3">
-        <v>22412</v>
+        <v>39102</v>
       </c>
       <c r="J3">
-        <v>29653</v>
+        <v>42224</v>
       </c>
       <c r="K3">
-        <v>11291</v>
+        <v>21567</v>
       </c>
       <c r="L3">
-        <v>30203</v>
+        <v>20670</v>
       </c>
       <c r="M3">
-        <v>9587</v>
+        <v>34543</v>
+      </c>
+      <c r="N3">
+        <v>14090</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4">
-        <v>15469.47</v>
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>4184</v>
       </c>
       <c r="D4">
-        <v>27398.35</v>
+        <v>25195.41</v>
       </c>
       <c r="E4">
-        <v>33968.93</v>
+        <v>21668.8</v>
       </c>
       <c r="F4">
-        <v>20246.74</v>
+        <v>12685.21</v>
       </c>
       <c r="G4">
-        <v>35681.74</v>
+        <v>17660.15</v>
       </c>
       <c r="H4">
-        <v>28733.48</v>
+        <v>22405.5</v>
       </c>
       <c r="I4">
-        <v>13960.25</v>
+        <v>27688.46</v>
       </c>
       <c r="J4">
-        <v>9124.67</v>
+        <v>27039.38</v>
       </c>
       <c r="K4">
-        <v>1937.81</v>
+        <v>17181.52</v>
       </c>
       <c r="L4">
-        <v>36594.04</v>
+        <v>4476.64</v>
       </c>
       <c r="M4">
-        <v>14140</v>
+        <v>20975.16</v>
+      </c>
+      <c r="N4">
+        <v>13303.24</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5">
-        <v>4174.84</v>
-      </c>
-      <c r="C5">
-        <v>13249.34</v>
+        <v>2015.63</v>
       </c>
       <c r="D5">
-        <v>11806.11</v>
+        <v>10714.45</v>
       </c>
       <c r="E5">
-        <v>20873.15</v>
+        <v>15683.31</v>
       </c>
       <c r="F5">
-        <v>28638.82</v>
+        <v>12347.43</v>
       </c>
       <c r="G5">
-        <v>19136.18</v>
+        <v>25470.56</v>
       </c>
       <c r="H5">
-        <v>29499.22</v>
+        <v>24511.52</v>
       </c>
       <c r="I5">
-        <v>18669.54</v>
+        <v>27061.47</v>
       </c>
       <c r="J5">
-        <v>14541.7</v>
+        <v>23394.93</v>
       </c>
       <c r="K5">
-        <v>12632.51</v>
+        <v>13715.08</v>
       </c>
       <c r="L5">
-        <v>17433.74</v>
+        <v>19022.35</v>
       </c>
       <c r="M5">
-        <v>7983.09</v>
+        <v>13591.65</v>
+      </c>
+      <c r="N5">
+        <v>17715.7</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>4016.26</v>
       </c>
       <c r="C6">
-        <v>28170.45</v>
+        <v>38.32</v>
       </c>
       <c r="D6">
-        <v>1441.23</v>
+        <v>17101.34</v>
       </c>
       <c r="E6">
-        <v>15144.11</v>
+        <v>16513.37</v>
       </c>
       <c r="F6">
-        <v>31491.82</v>
+        <v>15573.39</v>
       </c>
       <c r="G6">
-        <v>33434.98</v>
+        <v>16132.37</v>
       </c>
       <c r="H6">
-        <v>21784.95</v>
+        <v>37451.12</v>
       </c>
       <c r="I6">
-        <v>23786.16</v>
+        <v>28328.85</v>
       </c>
       <c r="J6">
-        <v>9036.059999999999</v>
+        <v>25673.88</v>
       </c>
       <c r="K6">
-        <v>4823.23</v>
+        <v>17992.67</v>
       </c>
       <c r="L6">
-        <v>21950.02</v>
+        <v>6873.47</v>
       </c>
       <c r="M6">
-        <v>14040.67</v>
+        <v>20044.31</v>
+      </c>
+      <c r="N6">
+        <v>7007.16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>